<commit_message>
updates session 3 and time-series resources
</commit_message>
<xml_diff>
--- a/project_morbius/pm_order_flow.xlsx
+++ b/project_morbius/pm_order_flow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\project_morbius\project_morbius\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3CCADA66-8D88-41D8-91A9-1628305ECD5A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FB7BEC9-FB3C-4DFF-8632-CA2F88362464}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20370" yWindow="-3765" windowWidth="29040" windowHeight="15840" xr2:uid="{FEC92D2C-8508-4B31-A66A-F6692FFF9B7F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{FEC92D2C-8508-4B31-A66A-F6692FFF9B7F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>Project Morbius Process Flow</t>
   </si>
@@ -47,6 +47,9 @@
   </si>
   <si>
     <t>Trade Test</t>
+  </si>
+  <si>
+    <t>Stage 2 - Pairs Trading</t>
   </si>
 </sst>
 </file>
@@ -1605,6 +1608,753 @@
 </file>
 
 <file path=xl/diagrams/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:colorsDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_2">
+  <dgm:title val=""/>
+  <dgm:desc val=""/>
+  <dgm:catLst>
+    <dgm:cat type="accent1" pri="11200"/>
+  </dgm:catLst>
+  <dgm:styleLbl name="node0">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="lnNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="vennNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgImgPlace1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgSibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgSibTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans1D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="callout">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst0">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst/>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="60000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="conFgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trAlignAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidFgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidAlignAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidBgAcc1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAccFollowNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAccFollowNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAccFollowNode1">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:alpha val="90000"/>
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc0">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc2">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc3">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc4">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="90000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="dkBgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:shade val="80000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trBgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="50000"/>
+        <a:alpha val="40000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="accent1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgShp">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="accent1">
+        <a:tint val="60000"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="lt1"/>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="dk1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="revTx">
+    <dgm:fillClrLst meth="repeat">
+      <a:schemeClr val="lt1">
+        <a:alpha val="0"/>
+      </a:schemeClr>
+    </dgm:fillClrLst>
+    <dgm:linClrLst meth="repeat">
+      <a:schemeClr val="dk1">
+        <a:alpha val="0"/>
+      </a:schemeClr>
+    </dgm:linClrLst>
+    <dgm:effectClrLst/>
+    <dgm:txLinClrLst/>
+    <dgm:txFillClrLst meth="repeat">
+      <a:schemeClr val="tx1"/>
+    </dgm:txFillClrLst>
+    <dgm:txEffectClrLst/>
+  </dgm:styleLbl>
+</dgm:colorsDef>
+</file>
+
+<file path=xl/diagrams/colors4.xml><?xml version="1.0" encoding="utf-8"?>
 <dgm:colorsDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_2">
   <dgm:title val=""/>
   <dgm:desc val=""/>
@@ -3983,6 +4733,641 @@
 </dgm:dataModel>
 </file>
 
+<file path=xl/diagrams/data4.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:dataModel xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <dgm:ptLst>
+    <dgm:pt modelId="{E101D2E7-A7F3-4C17-AC00-EBB9A5AFB075}" type="doc">
+      <dgm:prSet loTypeId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3" loCatId="hierarchy" qsTypeId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple1" qsCatId="simple" csTypeId="urn:microsoft.com/office/officeart/2005/8/colors/accent1_2" csCatId="accent1" phldr="1"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{2B8AD30E-7926-44D0-9333-2FB3D50B69D3}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Screen for 2 candidate stocks</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{4997EE32-04BB-46E9-A8CB-D3614EE06C08}" type="parTrans" cxnId="{45816304-4A90-44E9-9912-72A0A4BFDD17}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{24EECF7C-EFA2-49F7-8FD8-2091CFBE445C}" type="sibTrans" cxnId="{45816304-4A90-44E9-9912-72A0A4BFDD17}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{26FB135A-B404-4E10-861B-88ADCAF4266E}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>x criteria</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{60214CC3-84BD-495C-B0A6-F6F4A40DB64A}" type="parTrans" cxnId="{3B7A4256-C2E5-4664-A75B-2CFBCE196CB4}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{B4FB96BA-3227-4F11-A8F0-75C695EB444D}" type="sibTrans" cxnId="{3B7A4256-C2E5-4664-A75B-2CFBCE196CB4}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{8FF60D66-8570-4486-BAD1-63C6BC95B057}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>bruteforce</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{DCA21277-7621-412C-A8CA-6FC578F51011}" type="parTrans" cxnId="{607533F0-EFCA-47A5-81BD-C3802D4CB908}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{0AF93029-134C-40CE-A9A2-EA35B0A71DBB}" type="sibTrans" cxnId="{607533F0-EFCA-47A5-81BD-C3802D4CB908}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{A8EC609F-6D72-4F67-A2B0-6033250EDFAF}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Test both for stationarity</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{650020B9-DB37-4867-A6A8-4BE51100033B}" type="parTrans" cxnId="{B5A8BC4C-CEA7-4625-A594-5395F5B6CF6F}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{6CDFA299-9B59-4899-9529-BFB0E950B923}" type="sibTrans" cxnId="{B5A8BC4C-CEA7-4625-A594-5395F5B6CF6F}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{C3B1988B-CBFC-4592-9063-B0A60881B930}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Cure both by differencing to x order</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{87CE9753-C96A-4442-B2A7-680A6364CA58}" type="parTrans" cxnId="{D3C5AA2E-C2FF-40F8-9F26-48B5FC9215C3}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{38D9571D-0784-4C18-BA8B-2427641964E3}" type="sibTrans" cxnId="{D3C5AA2E-C2FF-40F8-9F26-48B5FC9215C3}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{53632B65-F78F-41B6-9DE4-F9D7A0D91109}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Check P-value for significant differencing</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{AF90B767-80C7-432F-A89C-42D9D53C8834}" type="parTrans" cxnId="{3FFFEB78-C78C-49D0-9EF2-73C66005FC02}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{EB80EE27-308A-4FA8-BB1E-7F1652538FE6}" type="sibTrans" cxnId="{3FFFEB78-C78C-49D0-9EF2-73C66005FC02}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{3F8A226E-EA42-4AD4-AA49-A4A3D40CEA00}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>Cointegration Test</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{FAA317EF-E42A-4885-B501-BF60E2F51400}" type="parTrans" cxnId="{AF614DA5-ED23-476D-ADC6-E993D47EEE45}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{C63DFF28-5037-4B71-B3B5-8953B2212820}" type="sibTrans" cxnId="{AF614DA5-ED23-476D-ADC6-E993D47EEE45}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{8A46A3B7-C763-4D0F-8C4F-846420ECFFC2}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>If same proceed, if not dump</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{1878D347-3F2D-4102-B245-828A0CC5C43B}" type="parTrans" cxnId="{80C3B610-393B-49AF-A30E-5AAD295AA239}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{AFDDAC53-3A8A-43FB-944C-CDF04EB65966}" type="sibTrans" cxnId="{80C3B610-393B-49AF-A30E-5AAD295AA239}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{62AFC473-C446-4819-9259-43BC8B43BC00}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>If p-val...</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{A7A0F1A4-F561-4D89-B37F-1E885D006F60}" type="parTrans" cxnId="{06A2E23B-25B0-43C0-B9DF-7D9C96F5C14F}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{02DD8A00-A41F-4AC0-9BDD-5BBA463634B4}" type="sibTrans" cxnId="{06A2E23B-25B0-43C0-B9DF-7D9C96F5C14F}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{842B6122-2ABF-45EB-BF3F-B05D7691B9BD}">
+      <dgm:prSet phldrT="[Text]"/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:r>
+            <a:rPr lang="en-US"/>
+            <a:t>X criteria to ensure forecast is predictive future</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{3BE71D44-D01A-46E8-BF29-B84900028741}" type="parTrans" cxnId="{6AD88881-3E51-4161-AC6B-131D8548B4B7}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{982791ED-EE3A-4A22-9DB3-A58D6DE20470}" type="sibTrans" cxnId="{6AD88881-3E51-4161-AC6B-131D8548B4B7}">
+      <dgm:prSet/>
+      <dgm:spPr/>
+      <dgm:t>
+        <a:bodyPr/>
+        <a:lstStyle/>
+        <a:p>
+          <a:endParaRPr lang="bg-BG"/>
+        </a:p>
+      </dgm:t>
+    </dgm:pt>
+    <dgm:pt modelId="{D4A4D681-8EAA-47AC-AB61-0806A0CEDAE5}" type="pres">
+      <dgm:prSet presAssocID="{E101D2E7-A7F3-4C17-AC00-EBB9A5AFB075}" presName="diagram" presStyleCnt="0">
+        <dgm:presLayoutVars>
+          <dgm:chPref val="1"/>
+          <dgm:dir/>
+          <dgm:animOne val="branch"/>
+          <dgm:animLvl val="lvl"/>
+          <dgm:resizeHandles/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{DDE825F5-0322-4A2C-8CE7-710DE9EBC7F6}" type="pres">
+      <dgm:prSet presAssocID="{2B8AD30E-7926-44D0-9333-2FB3D50B69D3}" presName="root" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{A199BBD6-56FD-4D4B-9C5F-6D8D5D291F60}" type="pres">
+      <dgm:prSet presAssocID="{2B8AD30E-7926-44D0-9333-2FB3D50B69D3}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{528DE460-1E28-4494-B25D-A3BD73296570}" type="pres">
+      <dgm:prSet presAssocID="{2B8AD30E-7926-44D0-9333-2FB3D50B69D3}" presName="rootText" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{09E6A6EB-CD4C-4740-A589-97AD90C09E59}" type="pres">
+      <dgm:prSet presAssocID="{2B8AD30E-7926-44D0-9333-2FB3D50B69D3}" presName="rootConnector" presStyleLbl="node1" presStyleIdx="0" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{6B44E87E-70D9-448B-871E-ACDBEABEA717}" type="pres">
+      <dgm:prSet presAssocID="{2B8AD30E-7926-44D0-9333-2FB3D50B69D3}" presName="childShape" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{9EA2A74A-09F2-4DEB-8A16-946828DF6C6E}" type="pres">
+      <dgm:prSet presAssocID="{60214CC3-84BD-495C-B0A6-F6F4A40DB64A}" presName="Name13" presStyleLbl="parChTrans1D2" presStyleIdx="0" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{1660CD49-D459-4781-9638-1E97CC0114A6}" type="pres">
+      <dgm:prSet presAssocID="{26FB135A-B404-4E10-861B-88ADCAF4266E}" presName="childText" presStyleLbl="bgAcc1" presStyleIdx="0" presStyleCnt="5">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{5074F93B-67C8-44EE-8C2F-12C7A6573B68}" type="pres">
+      <dgm:prSet presAssocID="{DCA21277-7621-412C-A8CA-6FC578F51011}" presName="Name13" presStyleLbl="parChTrans1D2" presStyleIdx="1" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{747E4B45-20CD-4288-9286-2E47688AADBB}" type="pres">
+      <dgm:prSet presAssocID="{8FF60D66-8570-4486-BAD1-63C6BC95B057}" presName="childText" presStyleLbl="bgAcc1" presStyleIdx="1" presStyleCnt="5">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{73955CCE-3095-430C-9709-A109D92EE710}" type="pres">
+      <dgm:prSet presAssocID="{A8EC609F-6D72-4F67-A2B0-6033250EDFAF}" presName="root" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{6975AB2C-B31E-4BAC-B671-360847C069B5}" type="pres">
+      <dgm:prSet presAssocID="{A8EC609F-6D72-4F67-A2B0-6033250EDFAF}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{80C09D3D-6668-45C3-A773-A98ABF145347}" type="pres">
+      <dgm:prSet presAssocID="{A8EC609F-6D72-4F67-A2B0-6033250EDFAF}" presName="rootText" presStyleLbl="node1" presStyleIdx="1" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{65D63A64-11C9-4EF2-8243-96454C89E97E}" type="pres">
+      <dgm:prSet presAssocID="{A8EC609F-6D72-4F67-A2B0-6033250EDFAF}" presName="rootConnector" presStyleLbl="node1" presStyleIdx="1" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{BE4C257B-249D-4214-A34C-82A018E27FDE}" type="pres">
+      <dgm:prSet presAssocID="{A8EC609F-6D72-4F67-A2B0-6033250EDFAF}" presName="childShape" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{F79FE8F8-F889-49AB-B1E4-D97E7C93543D}" type="pres">
+      <dgm:prSet presAssocID="{87CE9753-C96A-4442-B2A7-680A6364CA58}" presName="Name13" presStyleLbl="parChTrans1D2" presStyleIdx="2" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{C01FCEC5-378C-40AF-816A-E63EA32EF740}" type="pres">
+      <dgm:prSet presAssocID="{C3B1988B-CBFC-4592-9063-B0A60881B930}" presName="childText" presStyleLbl="bgAcc1" presStyleIdx="2" presStyleCnt="5">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{44B6884E-CFD3-4D1F-AD6D-54369E2E23BA}" type="pres">
+      <dgm:prSet presAssocID="{53632B65-F78F-41B6-9DE4-F9D7A0D91109}" presName="root" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{B3CFA645-7721-49D9-AC56-DAB287E89E8E}" type="pres">
+      <dgm:prSet presAssocID="{53632B65-F78F-41B6-9DE4-F9D7A0D91109}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{28C93417-C016-48B7-AC71-2DA5D9EB586D}" type="pres">
+      <dgm:prSet presAssocID="{53632B65-F78F-41B6-9DE4-F9D7A0D91109}" presName="rootText" presStyleLbl="node1" presStyleIdx="2" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{8CA29E5B-0BA8-41B9-83EC-806C88F9E1B7}" type="pres">
+      <dgm:prSet presAssocID="{53632B65-F78F-41B6-9DE4-F9D7A0D91109}" presName="rootConnector" presStyleLbl="node1" presStyleIdx="2" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{D3EA3A64-6F20-427A-AE77-EA09C56A8F1D}" type="pres">
+      <dgm:prSet presAssocID="{53632B65-F78F-41B6-9DE4-F9D7A0D91109}" presName="childShape" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{E1778CE1-B9A2-4E84-8A0D-51182BF54852}" type="pres">
+      <dgm:prSet presAssocID="{1878D347-3F2D-4102-B245-828A0CC5C43B}" presName="Name13" presStyleLbl="parChTrans1D2" presStyleIdx="3" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{DEF8742D-0F50-45D0-83E3-41F0841F8DC0}" type="pres">
+      <dgm:prSet presAssocID="{8A46A3B7-C763-4D0F-8C4F-846420ECFFC2}" presName="childText" presStyleLbl="bgAcc1" presStyleIdx="3" presStyleCnt="5">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{6D57597E-B72D-4C7A-BB0A-40C0A68EC713}" type="pres">
+      <dgm:prSet presAssocID="{3F8A226E-EA42-4AD4-AA49-A4A3D40CEA00}" presName="root" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{1622BE5A-E3F9-4AED-B6FB-6C007DCFD7C5}" type="pres">
+      <dgm:prSet presAssocID="{3F8A226E-EA42-4AD4-AA49-A4A3D40CEA00}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{D6B01640-D2BD-40F5-AA8F-4E29C0032112}" type="pres">
+      <dgm:prSet presAssocID="{3F8A226E-EA42-4AD4-AA49-A4A3D40CEA00}" presName="rootText" presStyleLbl="node1" presStyleIdx="3" presStyleCnt="5" custLinFactNeighborX="-1408"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{0AAD1A49-B5CA-4231-A486-E6378FBF3393}" type="pres">
+      <dgm:prSet presAssocID="{3F8A226E-EA42-4AD4-AA49-A4A3D40CEA00}" presName="rootConnector" presStyleLbl="node1" presStyleIdx="3" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{3338D736-690E-41E3-BBF8-845A14AFDB0D}" type="pres">
+      <dgm:prSet presAssocID="{3F8A226E-EA42-4AD4-AA49-A4A3D40CEA00}" presName="childShape" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{B5F0A462-AD43-4C90-B213-353D74849575}" type="pres">
+      <dgm:prSet presAssocID="{A7A0F1A4-F561-4D89-B37F-1E885D006F60}" presName="Name13" presStyleLbl="parChTrans1D2" presStyleIdx="4" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{FA64EC03-D566-49B5-BAF4-819EB9A09DC8}" type="pres">
+      <dgm:prSet presAssocID="{62AFC473-C446-4819-9259-43BC8B43BC00}" presName="childText" presStyleLbl="bgAcc1" presStyleIdx="4" presStyleCnt="5">
+        <dgm:presLayoutVars>
+          <dgm:bulletEnabled val="1"/>
+        </dgm:presLayoutVars>
+      </dgm:prSet>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{0B45EE39-B0B9-4E94-AB7E-8E33842FD7AD}" type="pres">
+      <dgm:prSet presAssocID="{842B6122-2ABF-45EB-BF3F-B05D7691B9BD}" presName="root" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{72A57B35-FE71-4686-AA05-E2AC7F8DCB19}" type="pres">
+      <dgm:prSet presAssocID="{842B6122-2ABF-45EB-BF3F-B05D7691B9BD}" presName="rootComposite" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{327FAE58-55E5-4A67-9EF6-1A3366895BD1}" type="pres">
+      <dgm:prSet presAssocID="{842B6122-2ABF-45EB-BF3F-B05D7691B9BD}" presName="rootText" presStyleLbl="node1" presStyleIdx="4" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{204C0F4D-19CD-4636-9923-9D8BCD2F0DE0}" type="pres">
+      <dgm:prSet presAssocID="{842B6122-2ABF-45EB-BF3F-B05D7691B9BD}" presName="rootConnector" presStyleLbl="node1" presStyleIdx="4" presStyleCnt="5"/>
+      <dgm:spPr/>
+    </dgm:pt>
+    <dgm:pt modelId="{FE23516D-6604-4799-A5FB-A60D3E163195}" type="pres">
+      <dgm:prSet presAssocID="{842B6122-2ABF-45EB-BF3F-B05D7691B9BD}" presName="childShape" presStyleCnt="0"/>
+      <dgm:spPr/>
+    </dgm:pt>
+  </dgm:ptLst>
+  <dgm:cxnLst>
+    <dgm:cxn modelId="{32D50C01-C1B4-474B-8E55-666CF5C6D3A7}" type="presOf" srcId="{26FB135A-B404-4E10-861B-88ADCAF4266E}" destId="{1660CD49-D459-4781-9638-1E97CC0114A6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{85B69A03-67B2-4704-A521-249BFEA852A1}" type="presOf" srcId="{842B6122-2ABF-45EB-BF3F-B05D7691B9BD}" destId="{204C0F4D-19CD-4636-9923-9D8BCD2F0DE0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{45816304-4A90-44E9-9912-72A0A4BFDD17}" srcId="{E101D2E7-A7F3-4C17-AC00-EBB9A5AFB075}" destId="{2B8AD30E-7926-44D0-9333-2FB3D50B69D3}" srcOrd="0" destOrd="0" parTransId="{4997EE32-04BB-46E9-A8CB-D3614EE06C08}" sibTransId="{24EECF7C-EFA2-49F7-8FD8-2091CFBE445C}"/>
+    <dgm:cxn modelId="{80C3B610-393B-49AF-A30E-5AAD295AA239}" srcId="{53632B65-F78F-41B6-9DE4-F9D7A0D91109}" destId="{8A46A3B7-C763-4D0F-8C4F-846420ECFFC2}" srcOrd="0" destOrd="0" parTransId="{1878D347-3F2D-4102-B245-828A0CC5C43B}" sibTransId="{AFDDAC53-3A8A-43FB-944C-CDF04EB65966}"/>
+    <dgm:cxn modelId="{1049EE28-9AD6-4557-BC1B-F90F41B4742D}" type="presOf" srcId="{60214CC3-84BD-495C-B0A6-F6F4A40DB64A}" destId="{9EA2A74A-09F2-4DEB-8A16-946828DF6C6E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{D3C5AA2E-C2FF-40F8-9F26-48B5FC9215C3}" srcId="{A8EC609F-6D72-4F67-A2B0-6033250EDFAF}" destId="{C3B1988B-CBFC-4592-9063-B0A60881B930}" srcOrd="0" destOrd="0" parTransId="{87CE9753-C96A-4442-B2A7-680A6364CA58}" sibTransId="{38D9571D-0784-4C18-BA8B-2427641964E3}"/>
+    <dgm:cxn modelId="{6ACBD52F-2097-4A20-801E-80C70B31B4E3}" type="presOf" srcId="{A7A0F1A4-F561-4D89-B37F-1E885D006F60}" destId="{B5F0A462-AD43-4C90-B213-353D74849575}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{CD0C5535-0AA6-463E-A6FA-79AA10E4CA3F}" type="presOf" srcId="{3F8A226E-EA42-4AD4-AA49-A4A3D40CEA00}" destId="{0AAD1A49-B5CA-4231-A486-E6378FBF3393}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{06A2E23B-25B0-43C0-B9DF-7D9C96F5C14F}" srcId="{3F8A226E-EA42-4AD4-AA49-A4A3D40CEA00}" destId="{62AFC473-C446-4819-9259-43BC8B43BC00}" srcOrd="0" destOrd="0" parTransId="{A7A0F1A4-F561-4D89-B37F-1E885D006F60}" sibTransId="{02DD8A00-A41F-4AC0-9BDD-5BBA463634B4}"/>
+    <dgm:cxn modelId="{1428663C-A009-475D-A1E4-6EED838D6057}" type="presOf" srcId="{1878D347-3F2D-4102-B245-828A0CC5C43B}" destId="{E1778CE1-B9A2-4E84-8A0D-51182BF54852}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{1028435C-F105-4D45-A1BA-E574AAD4523C}" type="presOf" srcId="{DCA21277-7621-412C-A8CA-6FC578F51011}" destId="{5074F93B-67C8-44EE-8C2F-12C7A6573B68}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{12484943-AC56-47DB-8706-701351441F50}" type="presOf" srcId="{62AFC473-C446-4819-9259-43BC8B43BC00}" destId="{FA64EC03-D566-49B5-BAF4-819EB9A09DC8}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{B5A8BC4C-CEA7-4625-A594-5395F5B6CF6F}" srcId="{E101D2E7-A7F3-4C17-AC00-EBB9A5AFB075}" destId="{A8EC609F-6D72-4F67-A2B0-6033250EDFAF}" srcOrd="1" destOrd="0" parTransId="{650020B9-DB37-4867-A6A8-4BE51100033B}" sibTransId="{6CDFA299-9B59-4899-9529-BFB0E950B923}"/>
+    <dgm:cxn modelId="{C8B4CE4D-0447-4330-A6E7-28E4C360C72B}" type="presOf" srcId="{2B8AD30E-7926-44D0-9333-2FB3D50B69D3}" destId="{09E6A6EB-CD4C-4740-A589-97AD90C09E59}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{3B7A4256-C2E5-4664-A75B-2CFBCE196CB4}" srcId="{2B8AD30E-7926-44D0-9333-2FB3D50B69D3}" destId="{26FB135A-B404-4E10-861B-88ADCAF4266E}" srcOrd="0" destOrd="0" parTransId="{60214CC3-84BD-495C-B0A6-F6F4A40DB64A}" sibTransId="{B4FB96BA-3227-4F11-A8F0-75C695EB444D}"/>
+    <dgm:cxn modelId="{37A75B57-3F9C-4E3B-B54A-C8993A7381D2}" type="presOf" srcId="{3F8A226E-EA42-4AD4-AA49-A4A3D40CEA00}" destId="{D6B01640-D2BD-40F5-AA8F-4E29C0032112}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{3FFFEB78-C78C-49D0-9EF2-73C66005FC02}" srcId="{E101D2E7-A7F3-4C17-AC00-EBB9A5AFB075}" destId="{53632B65-F78F-41B6-9DE4-F9D7A0D91109}" srcOrd="2" destOrd="0" parTransId="{AF90B767-80C7-432F-A89C-42D9D53C8834}" sibTransId="{EB80EE27-308A-4FA8-BB1E-7F1652538FE6}"/>
+    <dgm:cxn modelId="{6AD88881-3E51-4161-AC6B-131D8548B4B7}" srcId="{E101D2E7-A7F3-4C17-AC00-EBB9A5AFB075}" destId="{842B6122-2ABF-45EB-BF3F-B05D7691B9BD}" srcOrd="4" destOrd="0" parTransId="{3BE71D44-D01A-46E8-BF29-B84900028741}" sibTransId="{982791ED-EE3A-4A22-9DB3-A58D6DE20470}"/>
+    <dgm:cxn modelId="{84D00F9A-FBD8-4852-B3FE-31346B0747CC}" type="presOf" srcId="{A8EC609F-6D72-4F67-A2B0-6033250EDFAF}" destId="{65D63A64-11C9-4EF2-8243-96454C89E97E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{AF614DA5-ED23-476D-ADC6-E993D47EEE45}" srcId="{E101D2E7-A7F3-4C17-AC00-EBB9A5AFB075}" destId="{3F8A226E-EA42-4AD4-AA49-A4A3D40CEA00}" srcOrd="3" destOrd="0" parTransId="{FAA317EF-E42A-4885-B501-BF60E2F51400}" sibTransId="{C63DFF28-5037-4B71-B3B5-8953B2212820}"/>
+    <dgm:cxn modelId="{8ABE2AA8-1419-4ED6-BB57-6CCC3C6C8D5D}" type="presOf" srcId="{E101D2E7-A7F3-4C17-AC00-EBB9A5AFB075}" destId="{D4A4D681-8EAA-47AC-AB61-0806A0CEDAE5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{A3DF24B0-C01F-4789-AF36-043BEBD0DF9C}" type="presOf" srcId="{87CE9753-C96A-4442-B2A7-680A6364CA58}" destId="{F79FE8F8-F889-49AB-B1E4-D97E7C93543D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{007663B6-A854-4BA4-8982-05752EF329FB}" type="presOf" srcId="{8FF60D66-8570-4486-BAD1-63C6BC95B057}" destId="{747E4B45-20CD-4288-9286-2E47688AADBB}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{26B335BB-EAF5-420A-AB6D-A86ED5D5E7D7}" type="presOf" srcId="{2B8AD30E-7926-44D0-9333-2FB3D50B69D3}" destId="{528DE460-1E28-4494-B25D-A3BD73296570}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{5500E7BD-90E4-4894-A4FA-195DECF833E7}" type="presOf" srcId="{A8EC609F-6D72-4F67-A2B0-6033250EDFAF}" destId="{80C09D3D-6668-45C3-A773-A98ABF145347}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{AAC6D1CE-1AFF-45D0-AA8C-A5AB50D68B52}" type="presOf" srcId="{53632B65-F78F-41B6-9DE4-F9D7A0D91109}" destId="{28C93417-C016-48B7-AC71-2DA5D9EB586D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{0E693CDE-0291-410D-8D51-460A956C4BF0}" type="presOf" srcId="{8A46A3B7-C763-4D0F-8C4F-846420ECFFC2}" destId="{DEF8742D-0F50-45D0-83E3-41F0841F8DC0}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{58C067E0-EC04-46B8-87A0-6259FA9A36BA}" type="presOf" srcId="{53632B65-F78F-41B6-9DE4-F9D7A0D91109}" destId="{8CA29E5B-0BA8-41B9-83EC-806C88F9E1B7}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{8192F2E1-D88E-44E0-9068-1ADE5529776A}" type="presOf" srcId="{842B6122-2ABF-45EB-BF3F-B05D7691B9BD}" destId="{327FAE58-55E5-4A67-9EF6-1A3366895BD1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{607533F0-EFCA-47A5-81BD-C3802D4CB908}" srcId="{2B8AD30E-7926-44D0-9333-2FB3D50B69D3}" destId="{8FF60D66-8570-4486-BAD1-63C6BC95B057}" srcOrd="1" destOrd="0" parTransId="{DCA21277-7621-412C-A8CA-6FC578F51011}" sibTransId="{0AF93029-134C-40CE-A9A2-EA35B0A71DBB}"/>
+    <dgm:cxn modelId="{942138FB-8B99-4BF6-962F-A63815C72B57}" type="presOf" srcId="{C3B1988B-CBFC-4592-9063-B0A60881B930}" destId="{C01FCEC5-378C-40AF-816A-E63EA32EF740}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{69FC0FF9-72BA-4E6A-9A5B-9DCE9C336944}" type="presParOf" srcId="{D4A4D681-8EAA-47AC-AB61-0806A0CEDAE5}" destId="{DDE825F5-0322-4A2C-8CE7-710DE9EBC7F6}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{11BCABDC-42C8-435C-8457-5597538D5C42}" type="presParOf" srcId="{DDE825F5-0322-4A2C-8CE7-710DE9EBC7F6}" destId="{A199BBD6-56FD-4D4B-9C5F-6D8D5D291F60}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{AA29C8C4-E6A4-46F7-BD35-A49EEE6BF525}" type="presParOf" srcId="{A199BBD6-56FD-4D4B-9C5F-6D8D5D291F60}" destId="{528DE460-1E28-4494-B25D-A3BD73296570}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{CDB9905C-2447-40E1-BF40-CF91954325C0}" type="presParOf" srcId="{A199BBD6-56FD-4D4B-9C5F-6D8D5D291F60}" destId="{09E6A6EB-CD4C-4740-A589-97AD90C09E59}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{648B5361-4FD7-4609-8D11-2C6E76B23F71}" type="presParOf" srcId="{DDE825F5-0322-4A2C-8CE7-710DE9EBC7F6}" destId="{6B44E87E-70D9-448B-871E-ACDBEABEA717}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{6F6867BF-7800-4F38-B757-415B882BE4BD}" type="presParOf" srcId="{6B44E87E-70D9-448B-871E-ACDBEABEA717}" destId="{9EA2A74A-09F2-4DEB-8A16-946828DF6C6E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{92CEEB29-7F4F-44D9-BB73-27ADF5133B22}" type="presParOf" srcId="{6B44E87E-70D9-448B-871E-ACDBEABEA717}" destId="{1660CD49-D459-4781-9638-1E97CC0114A6}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{F3A34B68-B2AC-4FC3-A2F7-0A693FB4B3D0}" type="presParOf" srcId="{6B44E87E-70D9-448B-871E-ACDBEABEA717}" destId="{5074F93B-67C8-44EE-8C2F-12C7A6573B68}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{3BEE97B2-380B-452A-87C0-EC826CB6B36C}" type="presParOf" srcId="{6B44E87E-70D9-448B-871E-ACDBEABEA717}" destId="{747E4B45-20CD-4288-9286-2E47688AADBB}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{4E464027-B2CD-436E-B8C8-810E14C7BAF4}" type="presParOf" srcId="{D4A4D681-8EAA-47AC-AB61-0806A0CEDAE5}" destId="{73955CCE-3095-430C-9709-A109D92EE710}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{92E8DEA6-02F5-47E9-9FB8-604223059A65}" type="presParOf" srcId="{73955CCE-3095-430C-9709-A109D92EE710}" destId="{6975AB2C-B31E-4BAC-B671-360847C069B5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{F131E2C3-C088-4454-BC53-76D2B2B5BB8A}" type="presParOf" srcId="{6975AB2C-B31E-4BAC-B671-360847C069B5}" destId="{80C09D3D-6668-45C3-A773-A98ABF145347}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{937D4E57-8415-4F47-888A-0644CE4BA45B}" type="presParOf" srcId="{6975AB2C-B31E-4BAC-B671-360847C069B5}" destId="{65D63A64-11C9-4EF2-8243-96454C89E97E}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{2E3EE23F-2DEF-4365-A4BB-92A10E19F143}" type="presParOf" srcId="{73955CCE-3095-430C-9709-A109D92EE710}" destId="{BE4C257B-249D-4214-A34C-82A018E27FDE}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{29FF1042-F1F2-45B4-A237-26211123A7E9}" type="presParOf" srcId="{BE4C257B-249D-4214-A34C-82A018E27FDE}" destId="{F79FE8F8-F889-49AB-B1E4-D97E7C93543D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{3AFC8A1E-CBDC-4D3B-9494-F42D3577CA27}" type="presParOf" srcId="{BE4C257B-249D-4214-A34C-82A018E27FDE}" destId="{C01FCEC5-378C-40AF-816A-E63EA32EF740}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{7F41B6C8-078D-449F-A911-2BC1BE6B638C}" type="presParOf" srcId="{D4A4D681-8EAA-47AC-AB61-0806A0CEDAE5}" destId="{44B6884E-CFD3-4D1F-AD6D-54369E2E23BA}" srcOrd="2" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{DE306E40-FE88-4FBE-B7A6-980556057AD2}" type="presParOf" srcId="{44B6884E-CFD3-4D1F-AD6D-54369E2E23BA}" destId="{B3CFA645-7721-49D9-AC56-DAB287E89E8E}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{CF833717-70F6-498D-B864-D2FFA66F631E}" type="presParOf" srcId="{B3CFA645-7721-49D9-AC56-DAB287E89E8E}" destId="{28C93417-C016-48B7-AC71-2DA5D9EB586D}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{920907A6-8327-43B8-ABB8-8ADB50CC2C37}" type="presParOf" srcId="{B3CFA645-7721-49D9-AC56-DAB287E89E8E}" destId="{8CA29E5B-0BA8-41B9-83EC-806C88F9E1B7}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{09581FE7-717F-42DE-9045-2FC866F884FD}" type="presParOf" srcId="{44B6884E-CFD3-4D1F-AD6D-54369E2E23BA}" destId="{D3EA3A64-6F20-427A-AE77-EA09C56A8F1D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{06EF2AD9-2848-4EAC-A68F-637DC38BE387}" type="presParOf" srcId="{D3EA3A64-6F20-427A-AE77-EA09C56A8F1D}" destId="{E1778CE1-B9A2-4E84-8A0D-51182BF54852}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{BA81B47D-2306-4EE2-8BAD-AFDFAB87779D}" type="presParOf" srcId="{D3EA3A64-6F20-427A-AE77-EA09C56A8F1D}" destId="{DEF8742D-0F50-45D0-83E3-41F0841F8DC0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{55852969-6EC1-49C2-A51F-9378C8367C54}" type="presParOf" srcId="{D4A4D681-8EAA-47AC-AB61-0806A0CEDAE5}" destId="{6D57597E-B72D-4C7A-BB0A-40C0A68EC713}" srcOrd="3" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{FD362D8E-D59D-4E29-8AE3-7A235AA5C394}" type="presParOf" srcId="{6D57597E-B72D-4C7A-BB0A-40C0A68EC713}" destId="{1622BE5A-E3F9-4AED-B6FB-6C007DCFD7C5}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{90015948-B4BD-47C7-811A-F83F1B3A652A}" type="presParOf" srcId="{1622BE5A-E3F9-4AED-B6FB-6C007DCFD7C5}" destId="{D6B01640-D2BD-40F5-AA8F-4E29C0032112}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{D7F57EB9-669B-4846-8537-C7682DB62151}" type="presParOf" srcId="{1622BE5A-E3F9-4AED-B6FB-6C007DCFD7C5}" destId="{0AAD1A49-B5CA-4231-A486-E6378FBF3393}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{8D7FE900-80E8-49A8-907A-92437D8CA74C}" type="presParOf" srcId="{6D57597E-B72D-4C7A-BB0A-40C0A68EC713}" destId="{3338D736-690E-41E3-BBF8-845A14AFDB0D}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{EF7EFD10-BB9B-44EB-9C71-2AEC97DBA412}" type="presParOf" srcId="{3338D736-690E-41E3-BBF8-845A14AFDB0D}" destId="{B5F0A462-AD43-4C90-B213-353D74849575}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{A715B778-D7C0-48CA-9E02-B41B2FA111E1}" type="presParOf" srcId="{3338D736-690E-41E3-BBF8-845A14AFDB0D}" destId="{FA64EC03-D566-49B5-BAF4-819EB9A09DC8}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{9471C5B0-03B6-464D-AEF2-304F8C839EF0}" type="presParOf" srcId="{D4A4D681-8EAA-47AC-AB61-0806A0CEDAE5}" destId="{0B45EE39-B0B9-4E94-AB7E-8E33842FD7AD}" srcOrd="4" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{35925FCA-347A-43A7-B640-A9F166054793}" type="presParOf" srcId="{0B45EE39-B0B9-4E94-AB7E-8E33842FD7AD}" destId="{72A57B35-FE71-4686-AA05-E2AC7F8DCB19}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{A0E05132-3381-4DAA-8E71-DD106F5D6ADC}" type="presParOf" srcId="{72A57B35-FE71-4686-AA05-E2AC7F8DCB19}" destId="{327FAE58-55E5-4A67-9EF6-1A3366895BD1}" srcOrd="0" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{CA46B964-F747-48FD-92DB-BD62925FEA96}" type="presParOf" srcId="{72A57B35-FE71-4686-AA05-E2AC7F8DCB19}" destId="{204C0F4D-19CD-4636-9923-9D8BCD2F0DE0}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+    <dgm:cxn modelId="{2EA2315D-C60D-4391-A720-7D51F57E501F}" type="presParOf" srcId="{0B45EE39-B0B9-4E94-AB7E-8E33842FD7AD}" destId="{FE23516D-6604-4799-A5FB-A60D3E163195}" srcOrd="1" destOrd="0" presId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3"/>
+  </dgm:cxnLst>
+  <dgm:bg/>
+  <dgm:whole/>
+  <dgm:extLst>
+    <a:ext uri="http://schemas.microsoft.com/office/drawing/2008/diagram">
+      <dsp:dataModelExt xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" relId="rId20" minVer="http://schemas.openxmlformats.org/drawingml/2006/diagram"/>
+    </a:ext>
+  </dgm:extLst>
+</dgm:dataModel>
+</file>
+
 <file path=xl/diagrams/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <dsp:drawing xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <dsp:spTree>
@@ -7083,6 +8468,1118 @@
       <dsp:txXfrm>
         <a:off x="3993829" y="23373"/>
         <a:ext cx="1521159" cy="737630"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+  </dsp:spTree>
+</dsp:drawing>
+</file>
+
+<file path=xl/diagrams/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<dsp:drawing xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:dsp="http://schemas.microsoft.com/office/drawing/2008/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <dsp:spTree>
+    <dsp:nvGrpSpPr>
+      <dsp:cNvPr id="0" name=""/>
+      <dsp:cNvGrpSpPr/>
+    </dsp:nvGrpSpPr>
+    <dsp:grpSpPr/>
+    <dsp:sp modelId="{528DE460-1E28-4494-B25D-A3BD73296570}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3967" y="187886"/>
+          <a:ext cx="1352815" cy="676407"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="24765" tIns="16510" rIns="24765" bIns="16510" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300" kern="1200"/>
+            <a:t>Screen for 2 candidate stocks</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG" sz="1300" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="23778" y="207697"/>
+        <a:ext cx="1313193" cy="636785"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{9EA2A74A-09F2-4DEB-8A16-946828DF6C6E}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="139248" y="864294"/>
+          <a:ext cx="135281" cy="507305"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="0" y="507305"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="135281" y="507305"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{1660CD49-D459-4781-9638-1E97CC0114A6}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="274530" y="1033396"/>
+          <a:ext cx="1082252" cy="676407"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="26670" tIns="17780" rIns="26670" bIns="17780" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="622300">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200"/>
+            <a:t>x criteria</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG" sz="1400" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="294341" y="1053207"/>
+        <a:ext cx="1042630" cy="636785"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{5074F93B-67C8-44EE-8C2F-12C7A6573B68}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="139248" y="864294"/>
+          <a:ext cx="135281" cy="1352815"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="0" y="1352815"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="135281" y="1352815"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{747E4B45-20CD-4288-9286-2E47688AADBB}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="274530" y="1878905"/>
+          <a:ext cx="1082252" cy="676407"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="26670" tIns="17780" rIns="26670" bIns="17780" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="622300">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200"/>
+            <a:t>bruteforce</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG" sz="1400" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="294341" y="1898716"/>
+        <a:ext cx="1042630" cy="636785"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{80C09D3D-6668-45C3-A773-A98ABF145347}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="1694986" y="187886"/>
+          <a:ext cx="1352815" cy="676407"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="24765" tIns="16510" rIns="24765" bIns="16510" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300" kern="1200"/>
+            <a:t>Test both for stationarity</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG" sz="1300" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="1714797" y="207697"/>
+        <a:ext cx="1313193" cy="636785"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{F79FE8F8-F889-49AB-B1E4-D97E7C93543D}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="1830267" y="864294"/>
+          <a:ext cx="135281" cy="507305"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="0" y="507305"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="135281" y="507305"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{C01FCEC5-378C-40AF-816A-E63EA32EF740}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="1965549" y="1033396"/>
+          <a:ext cx="1082252" cy="676407"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="26670" tIns="17780" rIns="26670" bIns="17780" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="622300">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200"/>
+            <a:t>Cure both by differencing to x order</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG" sz="1400" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="1985360" y="1053207"/>
+        <a:ext cx="1042630" cy="636785"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{28C93417-C016-48B7-AC71-2DA5D9EB586D}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3386004" y="187886"/>
+          <a:ext cx="1352815" cy="676407"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="24765" tIns="16510" rIns="24765" bIns="16510" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300" kern="1200"/>
+            <a:t>Check P-value for significant differencing</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG" sz="1300" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3405815" y="207697"/>
+        <a:ext cx="1313193" cy="636785"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{E1778CE1-B9A2-4E84-8A0D-51182BF54852}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3521286" y="864294"/>
+          <a:ext cx="135281" cy="507305"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="0" y="507305"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="135281" y="507305"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{DEF8742D-0F50-45D0-83E3-41F0841F8DC0}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="3656567" y="1033396"/>
+          <a:ext cx="1082252" cy="676407"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="26670" tIns="17780" rIns="26670" bIns="17780" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="622300">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200"/>
+            <a:t>If same proceed, if not dump</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG" sz="1400" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="3676378" y="1053207"/>
+        <a:ext cx="1042630" cy="636785"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{D6B01640-D2BD-40F5-AA8F-4E29C0032112}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="5057976" y="187886"/>
+          <a:ext cx="1352815" cy="676407"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="24765" tIns="16510" rIns="24765" bIns="16510" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300" kern="1200"/>
+            <a:t>Cointegration Test</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG" sz="1300" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="5077787" y="207697"/>
+        <a:ext cx="1313193" cy="636785"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{B5F0A462-AD43-4C90-B213-353D74849575}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="5193257" y="864294"/>
+          <a:ext cx="154329" cy="507305"/>
+        </a:xfrm>
+        <a:custGeom>
+          <a:avLst/>
+          <a:gdLst/>
+          <a:ahLst/>
+          <a:cxnLst/>
+          <a:rect l="0" t="0" r="0" b="0"/>
+          <a:pathLst>
+            <a:path>
+              <a:moveTo>
+                <a:pt x="0" y="0"/>
+              </a:moveTo>
+              <a:lnTo>
+                <a:pt x="0" y="507305"/>
+              </a:lnTo>
+              <a:lnTo>
+                <a:pt x="154329" y="507305"/>
+              </a:lnTo>
+            </a:path>
+          </a:pathLst>
+        </a:custGeom>
+        <a:noFill/>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:shade val="60000"/>
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+    </dsp:sp>
+    <dsp:sp modelId="{FA64EC03-D566-49B5-BAF4-819EB9A09DC8}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="5347586" y="1033396"/>
+          <a:ext cx="1082252" cy="676407"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:alpha val="90000"/>
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="accent1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor"/>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="26670" tIns="17780" rIns="26670" bIns="17780" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="622300">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1400" kern="1200"/>
+            <a:t>If p-val...</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG" sz="1400" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="5367397" y="1053207"/>
+        <a:ext cx="1042630" cy="636785"/>
+      </dsp:txXfrm>
+    </dsp:sp>
+    <dsp:sp modelId="{327FAE58-55E5-4A67-9EF6-1A3366895BD1}">
+      <dsp:nvSpPr>
+        <dsp:cNvPr id="0" name=""/>
+        <dsp:cNvSpPr/>
+      </dsp:nvSpPr>
+      <dsp:spPr>
+        <a:xfrm>
+          <a:off x="6768042" y="187886"/>
+          <a:ext cx="1352815" cy="676407"/>
+        </a:xfrm>
+        <a:prstGeom prst="roundRect">
+          <a:avLst>
+            <a:gd name="adj" fmla="val 10000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="accent1">
+            <a:hueOff val="0"/>
+            <a:satOff val="0"/>
+            <a:lumOff val="0"/>
+            <a:alphaOff val="0"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="lt1">
+              <a:hueOff val="0"/>
+              <a:satOff val="0"/>
+              <a:lumOff val="0"/>
+              <a:alphaOff val="0"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:miter lim="800000"/>
+        </a:ln>
+        <a:effectLst/>
+      </dsp:spPr>
+      <dsp:style>
+        <a:lnRef idx="2">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </dsp:style>
+      <dsp:txBody>
+        <a:bodyPr spcFirstLastPara="0" vert="horz" wrap="square" lIns="24765" tIns="16510" rIns="24765" bIns="16510" numCol="1" spcCol="1270" anchor="ctr" anchorCtr="0">
+          <a:noAutofit/>
+        </a:bodyPr>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr marL="0" lvl="0" indent="0" algn="ctr" defTabSz="577850">
+            <a:lnSpc>
+              <a:spcPct val="90000"/>
+            </a:lnSpc>
+            <a:spcBef>
+              <a:spcPct val="0"/>
+            </a:spcBef>
+            <a:spcAft>
+              <a:spcPct val="35000"/>
+            </a:spcAft>
+            <a:buNone/>
+          </a:pPr>
+          <a:r>
+            <a:rPr lang="en-US" sz="1300" kern="1200"/>
+            <a:t>X criteria to ensure forecast is predictive future</a:t>
+          </a:r>
+          <a:endParaRPr lang="bg-BG" sz="1300" kern="1200"/>
+        </a:p>
+      </dsp:txBody>
+      <dsp:txXfrm>
+        <a:off x="6787853" y="207697"/>
+        <a:ext cx="1313193" cy="636785"/>
       </dsp:txXfrm>
     </dsp:sp>
   </dsp:spTree>
@@ -7819,6 +10316,298 @@
 </dgm:layoutDef>
 </file>
 
+<file path=xl/diagrams/layout4.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:layoutDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/layout/hierarchy3">
+  <dgm:title val=""/>
+  <dgm:desc val=""/>
+  <dgm:catLst>
+    <dgm:cat type="hierarchy" pri="7000"/>
+    <dgm:cat type="list" pri="23000"/>
+    <dgm:cat type="relationship" pri="15000"/>
+    <dgm:cat type="convert" pri="7000"/>
+  </dgm:catLst>
+  <dgm:sampData>
+    <dgm:dataModel>
+      <dgm:ptLst>
+        <dgm:pt modelId="0" type="doc"/>
+        <dgm:pt modelId="1">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="11">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="12">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="2">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="21">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+        <dgm:pt modelId="22">
+          <dgm:prSet phldr="1"/>
+        </dgm:pt>
+      </dgm:ptLst>
+      <dgm:cxnLst>
+        <dgm:cxn modelId="4" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="5" srcId="1" destId="11" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="6" srcId="1" destId="12" srcOrd="1" destOrd="0"/>
+        <dgm:cxn modelId="7" srcId="0" destId="2" srcOrd="1" destOrd="0"/>
+        <dgm:cxn modelId="8" srcId="2" destId="21" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="9" srcId="2" destId="22" srcOrd="1" destOrd="0"/>
+      </dgm:cxnLst>
+      <dgm:bg/>
+      <dgm:whole/>
+    </dgm:dataModel>
+  </dgm:sampData>
+  <dgm:styleData>
+    <dgm:dataModel>
+      <dgm:ptLst>
+        <dgm:pt modelId="0" type="doc"/>
+        <dgm:pt modelId="1"/>
+        <dgm:pt modelId="11"/>
+        <dgm:pt modelId="2"/>
+        <dgm:pt modelId="21"/>
+      </dgm:ptLst>
+      <dgm:cxnLst>
+        <dgm:cxn modelId="4" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="5" srcId="0" destId="2" srcOrd="1" destOrd="0"/>
+        <dgm:cxn modelId="13" srcId="1" destId="11" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="23" srcId="2" destId="21" srcOrd="0" destOrd="0"/>
+      </dgm:cxnLst>
+      <dgm:bg/>
+      <dgm:whole/>
+    </dgm:dataModel>
+  </dgm:styleData>
+  <dgm:clrData>
+    <dgm:dataModel>
+      <dgm:ptLst>
+        <dgm:pt modelId="0" type="doc"/>
+        <dgm:pt modelId="1"/>
+        <dgm:pt modelId="11"/>
+        <dgm:pt modelId="2"/>
+        <dgm:pt modelId="21"/>
+        <dgm:pt modelId="3"/>
+        <dgm:pt modelId="31"/>
+        <dgm:pt modelId="4"/>
+        <dgm:pt modelId="41"/>
+      </dgm:ptLst>
+      <dgm:cxnLst>
+        <dgm:cxn modelId="5" srcId="0" destId="1" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="6" srcId="0" destId="2" srcOrd="1" destOrd="0"/>
+        <dgm:cxn modelId="7" srcId="0" destId="3" srcOrd="2" destOrd="0"/>
+        <dgm:cxn modelId="8" srcId="0" destId="4" srcOrd="3" destOrd="0"/>
+        <dgm:cxn modelId="13" srcId="1" destId="11" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="23" srcId="2" destId="21" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="33" srcId="3" destId="31" srcOrd="0" destOrd="0"/>
+        <dgm:cxn modelId="43" srcId="4" destId="41" srcOrd="0" destOrd="0"/>
+      </dgm:cxnLst>
+      <dgm:bg/>
+      <dgm:whole/>
+    </dgm:dataModel>
+  </dgm:clrData>
+  <dgm:layoutNode name="diagram">
+    <dgm:varLst>
+      <dgm:chPref val="1"/>
+      <dgm:dir/>
+      <dgm:animOne val="branch"/>
+      <dgm:animLvl val="lvl"/>
+      <dgm:resizeHandles/>
+    </dgm:varLst>
+    <dgm:choose name="Name0">
+      <dgm:if name="Name1" func="var" arg="dir" op="equ" val="norm">
+        <dgm:alg type="hierChild">
+          <dgm:param type="linDir" val="fromL"/>
+        </dgm:alg>
+      </dgm:if>
+      <dgm:else name="Name2">
+        <dgm:alg type="hierChild">
+          <dgm:param type="linDir" val="fromR"/>
+        </dgm:alg>
+      </dgm:else>
+    </dgm:choose>
+    <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+      <dgm:adjLst/>
+    </dgm:shape>
+    <dgm:presOf/>
+    <dgm:constrLst>
+      <dgm:constr type="primFontSz" for="des" forName="rootText" op="equ" val="65"/>
+      <dgm:constr type="primFontSz" for="des" forName="childText" op="equ" val="65"/>
+      <dgm:constr type="w" for="des" forName="rootComposite" refType="w"/>
+      <dgm:constr type="h" for="des" forName="rootComposite" refType="w" fact="0.5"/>
+      <dgm:constr type="w" for="des" forName="childText" refType="w" refFor="des" refForName="rootComposite" fact="0.8"/>
+      <dgm:constr type="h" for="des" forName="childText" refType="h" refFor="des" refForName="rootComposite"/>
+      <dgm:constr type="sibSp" refType="w" refFor="des" refForName="rootComposite" fact="0.25"/>
+      <dgm:constr type="sibSp" for="des" forName="childShape" refType="h" refFor="des" refForName="childText" fact="0.25"/>
+      <dgm:constr type="sp" for="des" forName="root" refType="h" refFor="des" refForName="childText" fact="0.25"/>
+    </dgm:constrLst>
+    <dgm:ruleLst/>
+    <dgm:forEach name="Name3" axis="ch">
+      <dgm:forEach name="Name4" axis="self" ptType="node" cnt="1">
+        <dgm:layoutNode name="root">
+          <dgm:choose name="Name5">
+            <dgm:if name="Name6" func="var" arg="dir" op="equ" val="norm">
+              <dgm:alg type="hierRoot">
+                <dgm:param type="hierAlign" val="tL"/>
+              </dgm:alg>
+            </dgm:if>
+            <dgm:else name="Name7">
+              <dgm:alg type="hierRoot">
+                <dgm:param type="hierAlign" val="tR"/>
+              </dgm:alg>
+            </dgm:else>
+          </dgm:choose>
+          <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+            <dgm:adjLst/>
+          </dgm:shape>
+          <dgm:presOf/>
+          <dgm:constrLst>
+            <dgm:constr type="alignOff" val="0.2"/>
+          </dgm:constrLst>
+          <dgm:ruleLst/>
+          <dgm:layoutNode name="rootComposite">
+            <dgm:alg type="composite"/>
+            <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+              <dgm:adjLst/>
+            </dgm:shape>
+            <dgm:presOf axis="self" ptType="node" cnt="1"/>
+            <dgm:choose name="Name8">
+              <dgm:if name="Name9" func="var" arg="dir" op="equ" val="norm">
+                <dgm:constrLst>
+                  <dgm:constr type="l" for="ch" forName="rootText"/>
+                  <dgm:constr type="t" for="ch" forName="rootText"/>
+                  <dgm:constr type="w" for="ch" forName="rootText" refType="w"/>
+                  <dgm:constr type="h" for="ch" forName="rootText" refType="h"/>
+                  <dgm:constr type="l" for="ch" forName="rootConnector"/>
+                  <dgm:constr type="t" for="ch" forName="rootConnector"/>
+                  <dgm:constr type="w" for="ch" forName="rootConnector" refType="w" refFor="ch" refForName="rootText" fact="0.2"/>
+                  <dgm:constr type="h" for="ch" forName="rootConnector" refType="h" refFor="ch" refForName="rootText"/>
+                </dgm:constrLst>
+              </dgm:if>
+              <dgm:else name="Name10">
+                <dgm:constrLst>
+                  <dgm:constr type="l" for="ch" forName="rootText"/>
+                  <dgm:constr type="t" for="ch" forName="rootText"/>
+                  <dgm:constr type="w" for="ch" forName="rootText" refType="w"/>
+                  <dgm:constr type="h" for="ch" forName="rootText" refType="h"/>
+                  <dgm:constr type="r" for="ch" forName="rootConnector" refType="w"/>
+                  <dgm:constr type="t" for="ch" forName="rootConnector"/>
+                  <dgm:constr type="w" for="ch" forName="rootConnector" refType="w" refFor="ch" refForName="rootText" fact="0.2"/>
+                  <dgm:constr type="h" for="ch" forName="rootConnector" refType="h" refFor="ch" refForName="rootText"/>
+                </dgm:constrLst>
+              </dgm:else>
+            </dgm:choose>
+            <dgm:ruleLst/>
+            <dgm:layoutNode name="rootText" styleLbl="node1">
+              <dgm:alg type="tx"/>
+              <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="roundRect" r:blip="">
+                <dgm:adjLst>
+                  <dgm:adj idx="1" val="0.1"/>
+                </dgm:adjLst>
+              </dgm:shape>
+              <dgm:presOf axis="self" ptType="node" cnt="1"/>
+              <dgm:constrLst>
+                <dgm:constr type="tMarg" refType="primFontSz" fact="0.1"/>
+                <dgm:constr type="bMarg" refType="primFontSz" fact="0.1"/>
+                <dgm:constr type="lMarg" refType="primFontSz" fact="0.15"/>
+                <dgm:constr type="rMarg" refType="primFontSz" fact="0.15"/>
+              </dgm:constrLst>
+              <dgm:ruleLst>
+                <dgm:rule type="primFontSz" val="5" fact="NaN" max="NaN"/>
+              </dgm:ruleLst>
+            </dgm:layoutNode>
+            <dgm:layoutNode name="rootConnector" moveWith="rootText">
+              <dgm:alg type="sp"/>
+              <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="roundRect" r:blip="" hideGeom="1">
+                <dgm:adjLst>
+                  <dgm:adj idx="1" val="0.1"/>
+                </dgm:adjLst>
+              </dgm:shape>
+              <dgm:presOf axis="self" ptType="node" cnt="1"/>
+              <dgm:constrLst/>
+              <dgm:ruleLst/>
+            </dgm:layoutNode>
+          </dgm:layoutNode>
+          <dgm:layoutNode name="childShape">
+            <dgm:alg type="hierChild">
+              <dgm:param type="chAlign" val="l"/>
+              <dgm:param type="linDir" val="fromT"/>
+            </dgm:alg>
+            <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:blip="">
+              <dgm:adjLst/>
+            </dgm:shape>
+            <dgm:presOf/>
+            <dgm:constrLst/>
+            <dgm:ruleLst/>
+            <dgm:forEach name="Name11" axis="ch">
+              <dgm:forEach name="Name12" axis="self" ptType="parTrans" cnt="1">
+                <dgm:layoutNode name="Name13">
+                  <dgm:choose name="Name14">
+                    <dgm:if name="Name15" func="var" arg="dir" op="equ" val="norm">
+                      <dgm:alg type="conn">
+                        <dgm:param type="dim" val="1D"/>
+                        <dgm:param type="endSty" val="noArr"/>
+                        <dgm:param type="connRout" val="bend"/>
+                        <dgm:param type="srcNode" val="rootConnector"/>
+                        <dgm:param type="begPts" val="bCtr"/>
+                        <dgm:param type="endPts" val="midL"/>
+                      </dgm:alg>
+                    </dgm:if>
+                    <dgm:else name="Name16">
+                      <dgm:alg type="conn">
+                        <dgm:param type="dim" val="1D"/>
+                        <dgm:param type="endSty" val="noArr"/>
+                        <dgm:param type="connRout" val="bend"/>
+                        <dgm:param type="srcNode" val="rootConnector"/>
+                        <dgm:param type="begPts" val="bCtr"/>
+                        <dgm:param type="endPts" val="midR"/>
+                      </dgm:alg>
+                    </dgm:else>
+                  </dgm:choose>
+                  <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="conn" r:blip="">
+                    <dgm:adjLst/>
+                  </dgm:shape>
+                  <dgm:presOf axis="self"/>
+                  <dgm:constrLst>
+                    <dgm:constr type="begPad"/>
+                    <dgm:constr type="endPad"/>
+                  </dgm:constrLst>
+                  <dgm:ruleLst/>
+                </dgm:layoutNode>
+              </dgm:forEach>
+              <dgm:forEach name="Name17" axis="self" ptType="node">
+                <dgm:layoutNode name="childText" styleLbl="bgAcc1">
+                  <dgm:varLst>
+                    <dgm:bulletEnabled val="1"/>
+                  </dgm:varLst>
+                  <dgm:alg type="tx"/>
+                  <dgm:shape xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" type="roundRect" r:blip="">
+                    <dgm:adjLst>
+                      <dgm:adj idx="1" val="0.1"/>
+                    </dgm:adjLst>
+                  </dgm:shape>
+                  <dgm:presOf axis="self desOrSelf" ptType="node node" st="1 1" cnt="1 0"/>
+                  <dgm:constrLst>
+                    <dgm:constr type="tMarg" refType="primFontSz" fact="0.1"/>
+                    <dgm:constr type="bMarg" refType="primFontSz" fact="0.1"/>
+                    <dgm:constr type="lMarg" refType="primFontSz" fact="0.15"/>
+                    <dgm:constr type="rMarg" refType="primFontSz" fact="0.15"/>
+                  </dgm:constrLst>
+                  <dgm:ruleLst>
+                    <dgm:rule type="primFontSz" val="5" fact="NaN" max="NaN"/>
+                  </dgm:ruleLst>
+                </dgm:layoutNode>
+              </dgm:forEach>
+            </dgm:forEach>
+          </dgm:layoutNode>
+        </dgm:layoutNode>
+      </dgm:forEach>
+    </dgm:forEach>
+  </dgm:layoutNode>
+</dgm:layoutDef>
+</file>
+
 <file path=xl/diagrams/quickStyle1.xml><?xml version="1.0" encoding="utf-8"?>
 <dgm:styleDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple1">
   <dgm:title val=""/>
@@ -9888,6 +12677,1040 @@
 </file>
 
 <file path=xl/diagrams/quickStyle3.xml><?xml version="1.0" encoding="utf-8"?>
+<dgm:styleDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple1">
+  <dgm:title val=""/>
+  <dgm:desc val=""/>
+  <dgm:catLst>
+    <dgm:cat type="simple" pri="10100"/>
+  </dgm:catLst>
+  <dgm:scene3d>
+    <a:camera prst="orthographicFront"/>
+    <a:lightRig rig="threePt" dir="t"/>
+  </dgm:scene3d>
+  <dgm:styleLbl name="node0">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="lnNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="vennNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="tx1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="node4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgImgPlace1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignImgPlace1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgImgPlace1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgSibTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgSibTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="sibTrans1D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="callout">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst0">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="asst4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans2D4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor">
+        <a:schemeClr val="lt1"/>
+      </a:fontRef>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="parChTrans1D4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="conFgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trAlignAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidFgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidAlignAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="solidBgAcc1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAccFollowNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="alignAccFollowNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgAccFollowNode1">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc0">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc2">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc3">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgAcc4">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="bgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="dkBgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="trBgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="fgShp">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="2">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="1">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+  <dgm:styleLbl name="revTx">
+    <dgm:scene3d>
+      <a:camera prst="orthographicFront"/>
+      <a:lightRig rig="threePt" dir="t"/>
+    </dgm:scene3d>
+    <dgm:sp3d/>
+    <dgm:txPr/>
+    <dgm:style>
+      <a:lnRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:lnRef>
+      <a:fillRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:fillRef>
+      <a:effectRef idx="0">
+        <a:scrgbClr r="0" g="0" b="0"/>
+      </a:effectRef>
+      <a:fontRef idx="minor"/>
+    </dgm:style>
+  </dgm:styleLbl>
+</dgm:styleDef>
+</file>
+
+<file path=xl/diagrams/quickStyle4.xml><?xml version="1.0" encoding="utf-8"?>
 <dgm:styleDef xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" uniqueId="urn:microsoft.com/office/officeart/2005/8/quickstyle/simple1">
   <dgm:title val=""/>
   <dgm:desc val=""/>
@@ -11138,6 +14961,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/diagram">
           <dgm:relIds xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:dm="rId11" r:lo="rId12" r:qs="rId13" r:cs="rId14"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>2</xdr:col>
+      <xdr:colOff>476249</xdr:colOff>
+      <xdr:row>54</xdr:row>
+      <xdr:rowOff>166687</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>66674</xdr:colOff>
+      <xdr:row>67</xdr:row>
+      <xdr:rowOff>185737</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Diagram 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{590C5243-5814-9953-2AF2-EA6289B94891}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/diagram">
+          <dgm:relIds xmlns:dgm="http://schemas.openxmlformats.org/drawingml/2006/diagram" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:dm="rId16" r:lo="rId17" r:qs="rId18" r:cs="rId19"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -11443,10 +15302,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3D766006-7E30-4DDE-857D-644C6391CA3B}">
-  <dimension ref="A1:L41"/>
+  <dimension ref="A1:L59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
-      <selection activeCell="U31" sqref="U31"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="Q7" sqref="Q7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -11482,6 +15341,11 @@
         <v>3</v>
       </c>
     </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>4</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>